<commit_message>
Minor Clean Up and Exam 2 Start
Minor clean up items and put the beginnings of exam 2 in the repo.
</commit_message>
<xml_diff>
--- a/HW3/StatisticalAnalysis.xlsx
+++ b/HW3/StatisticalAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serial Run Time" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Parallel Run Time NP = 4" sheetId="6" r:id="rId4"/>
     <sheet name="Parallel Run Time NP = 8" sheetId="8" r:id="rId5"/>
     <sheet name="Parallel Relative Speedup" sheetId="9" r:id="rId6"/>
-    <sheet name="Data" sheetId="1" r:id="rId7"/>
+    <sheet name="Parallel Relative Efficiency" sheetId="10" r:id="rId7"/>
+    <sheet name="Data" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Serial</t>
   </si>
@@ -47,9 +48,6 @@
     <t>NP = 8</t>
   </si>
   <si>
-    <t>RelativeEfficiency</t>
-  </si>
-  <si>
     <t>RelativeSpeedup(NP=2)</t>
   </si>
   <si>
@@ -57,6 +55,15 @@
   </si>
   <si>
     <t>RelativeSpeedup(NP = 8)</t>
+  </si>
+  <si>
+    <t>RelativeEfficiency(NP=2)</t>
+  </si>
+  <si>
+    <t>RelativeEfficiency(NP=4)</t>
+  </si>
+  <si>
+    <t>RelativeEfficiency(NP=8)</t>
   </si>
 </sst>
 </file>
@@ -99,9 +106,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3948,6 +3956,868 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Relative Speed Up for Parallel Matrix Multiplication - Run on Jetson Cluster UAH</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.9495692828947728E-2"/>
+          <c:y val="7.4851744307535995E-2"/>
+          <c:w val="0.89922299298562236"/>
+          <c:h val="0.83553744446420175"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RelativeEfficiency(NP=2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2816</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3328</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$K$2:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.77013996666091855</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84462987070188988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0692579724817084</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95148466719973512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99460202625856131</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.955772965403065</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92708137117796463</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98257684818346513</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0043454228121536</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95718992067826025</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0020217612117954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.000887710821353</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98319950714833659</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90697864896115976</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91AC-470E-A85C-97163C3C5907}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RelativeEfficiency(NP=4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2816</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3328</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$L$2:$L$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.48993929753350524</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74513337455055384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95084649563248191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95861978349722687</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98182640165932422</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97433967781169128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93483959872315825</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94846887973828364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0050017081353493</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96757257586143597</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0060044073629986</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95027274447525678</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97570878018046647</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91166809449777353</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-91AC-470E-A85C-97163C3C5907}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RelativeEfficiency(NP=8)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2816</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3328</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$M$2:$M$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.31513136231065952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55004806123281524</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79942025285796658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91890957172646159</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96683564960190904</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95317097762499536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92281853187674379</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93758546056227121</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99495319475329214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94448230108332343</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98704525432180856</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9208408960152159</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.96716672186010166</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.92786370956346031</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-91AC-470E-A85C-97163C3C5907}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="621842496"/>
+        <c:axId val="621845448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="621842496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Matrix</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621845448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="621845448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="621842496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.65982402696503151"/>
+          <c:y val="0.37635501468056715"/>
+          <c:w val="0.17465484040030485"/>
+          <c:h val="0.10216759444164504"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4188,6 +5058,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6769,6 +7679,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7341,6 +8767,17 @@
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D87E95AC-7575-431A-98C2-C19603B852CD}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F25A8FC2-85F4-4747-85AC-637B48614AF4}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
@@ -7519,13 +8956,46 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6FCCCC-E35F-47BF-9353-F9D3401DE918}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
     <xdr:ext cx="8670192" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6FCCCC-E35F-47BF-9353-F9D3401DE918}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A60E4FB5-563E-4A10-839B-72B8F3C9E6CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7845,10 +9315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" activeCellId="3" sqref="A1:A1048576 G1:G1048576 H1:H1048576 I1:I1048576"/>
+      <selection activeCell="M1" activeCellId="3" sqref="A1:A1048576 K1:K1048576 L1:L1048576 M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7858,7 +9328,7 @@
     <col min="7" max="7" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -7879,22 +9349,22 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>5</v>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7926,16 +9396,16 @@
         <v>2.5210508984852762</v>
       </c>
       <c r="K2" s="1">
-        <f>C2/B2</f>
-        <v>0.64923263516350227</v>
+        <f>B2/(2*C2)</f>
+        <v>0.77013996666091855</v>
       </c>
       <c r="L2" s="1">
-        <f>D2/B2</f>
-        <v>0.51026729486402012</v>
+        <f>B2/(4*D2)</f>
+        <v>0.48993929753350524</v>
       </c>
       <c r="M2" s="1">
-        <f>E2/B2</f>
-        <v>0.39665998040770628</v>
+        <f>B2/(8*E2)</f>
+        <v>0.31513136231065952</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7967,16 +9437,16 @@
         <v>4.400384489862522</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K15" si="3">C3/B3</f>
-        <v>0.59197527502135172</v>
+        <f t="shared" ref="K3:K15" si="3">B3/(2*C3)</f>
+        <v>0.84462987070188988</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L15" si="4">D3/B3</f>
-        <v>0.33551040463164578</v>
+        <f t="shared" ref="L3:L15" si="4">B3/(4*D3)</f>
+        <v>0.74513337455055384</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M15" si="5">E3/B3</f>
-        <v>0.22725286899446423</v>
+        <f t="shared" ref="M3:M15" si="5">B3/(8*E3)</f>
+        <v>0.55004806123281524</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -8009,15 +9479,15 @@
       </c>
       <c r="K4" s="1">
         <f t="shared" si="3"/>
-        <v>0.46761400229686245</v>
+        <v>1.0692579724817084</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="4"/>
-        <v>0.26292361716462503</v>
+        <v>0.95084649563248191</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" si="5"/>
-        <v>0.15636331398049882</v>
+        <v>0.79942025285796658</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -8050,15 +9520,15 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" si="3"/>
-        <v>0.52549454261992889</v>
+        <v>0.95148466719973512</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="4"/>
-        <v>0.26079161342566137</v>
+        <v>0.95861978349722687</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="5"/>
-        <v>0.13603079546243932</v>
+        <v>0.91890957172646159</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -8091,15 +9561,15 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="3"/>
-        <v>0.5027136350011997</v>
+        <v>0.99460202625856131</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="4"/>
-        <v>0.25462749787283212</v>
+        <v>0.98182640165932422</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="5"/>
-        <v>0.12928774404571064</v>
+        <v>0.96683564960190904</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -8132,15 +9602,15 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="3"/>
-        <v>0.52313678885983328</v>
+        <v>0.955772965403065</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="4"/>
-        <v>0.25658402884863019</v>
+        <v>0.97433967781169128</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" si="5"/>
-        <v>0.13114121488619071</v>
+        <v>0.95317097762499536</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -8173,15 +9643,15 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="3"/>
-        <v>0.53932698417258873</v>
+        <v>0.92708137117796463</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="4"/>
-        <v>0.26742555657832651</v>
+        <v>0.93483959872315825</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" si="5"/>
-        <v>0.13545458362846968</v>
+        <v>0.92281853187674379</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -8214,15 +9684,15 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="3"/>
-        <v>0.50886605045129341</v>
+        <v>0.98257684818346513</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="4"/>
-        <v>0.26358271245439691</v>
+        <v>0.94846887973828364</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="5"/>
-        <v>0.13332118005012294</v>
+        <v>0.93758546056227121</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -8255,15 +9725,15 @@
       </c>
       <c r="K10" s="1">
         <f t="shared" si="3"/>
-        <v>0.49783668909448187</v>
+        <v>1.0043454228121536</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="4"/>
-        <v>0.24875579611087695</v>
+        <v>1.0050017081353493</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" si="5"/>
-        <v>0.12563405058566088</v>
+        <v>0.99495319475329214</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -8296,15 +9766,15 @@
       </c>
       <c r="K11" s="1">
         <f t="shared" si="3"/>
-        <v>0.52236237469540248</v>
+        <v>0.95718992067826025</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="4"/>
-        <v>0.25837855085694572</v>
+        <v>0.96757257586143597</v>
       </c>
       <c r="M11" s="1">
         <f t="shared" si="5"/>
-        <v>0.13234763621999554</v>
+        <v>0.94448230108332343</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -8337,15 +9807,15 @@
       </c>
       <c r="K12" s="1">
         <f t="shared" si="3"/>
-        <v>0.49899115902964508</v>
+        <v>1.0020217612117954</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="4"/>
-        <v>0.24850785759012289</v>
+        <v>1.0060044073629986</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="5"/>
-        <v>0.12664059672308192</v>
+        <v>0.98704525432180856</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -8378,15 +9848,15 @@
       </c>
       <c r="K13" s="1">
         <f t="shared" si="3"/>
-        <v>0.49955653825511331</v>
+        <v>1.000887710821353</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="4"/>
-        <v>0.26308236393547274</v>
+        <v>0.95027274447525678</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" si="5"/>
-        <v>0.13574549147514675</v>
+        <v>0.9208408960152159</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -8419,15 +9889,15 @@
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v>0.50854378624557661</v>
+        <v>0.98319950714833659</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="4"/>
-        <v>0.25622399334539159</v>
+        <v>0.97570878018046647</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" si="5"/>
-        <v>0.12924348736854177</v>
+        <v>0.96716672186010166</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -8460,16 +9930,58 @@
       </c>
       <c r="K15" s="1">
         <f t="shared" si="3"/>
-        <v>0.55128089351683507</v>
+        <v>0.90697864896115976</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="4"/>
-        <v>0.27422260525385816</v>
+        <v>0.91166809449777353</v>
       </c>
       <c r="M15" s="1">
         <f t="shared" si="5"/>
-        <v>0.13471806118897545</v>
-      </c>
+        <v>0.92786370956346031</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>